<commit_message>
changes on download history user
</commit_message>
<xml_diff>
--- a/public/xlsx/user/5fcccc7ca137ca27fb71127a.xlsx
+++ b/public/xlsx/user/5fcccc7ca137ca27fb71127a.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,9 +450,29 @@
 dg</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>5fef0a8c7682981e94fcf376</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Jhon Deo</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Fri Jan 01 2021</v>
+      </c>
+      <c r="D4" t="str">
+        <v>5:20 PM-5:35 PM</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Paracetamol</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Take medicine 3 times after food</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>